<commit_message>
chore: update business planning documents and cost lists
🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/docs/business/Comprehensive_Cost_List.xlsx
+++ b/docs/business/Comprehensive_Cost_List.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/max/Development/active/being/development/docs/business/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE8D7B26-43F8-F84D-805E-CF4666F780F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72BA3CF6-E691-4C47-BB01-A0DF3B0E7361}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="38400" windowHeight="24100" xr2:uid="{688B0B1E-5751-5042-B68D-FFC82480E3B2}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="22140" windowHeight="24100" xr2:uid="{688B0B1E-5751-5042-B68D-FFC82480E3B2}"/>
   </bookViews>
   <sheets>
     <sheet name="Comprehensive_Cost_List_Final" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Comprehensive_Cost_List_Final!$A$7:$K$105</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Comprehensive_Cost_List_Final!$A$7:$K$101</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="738" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="698" uniqueCount="253">
   <si>
     <t>CONFIDENCE LEVEL DEFINITIONS</t>
   </si>
@@ -260,9 +260,6 @@
     <t>Premeditatio Malorum Safety Validation</t>
   </si>
   <si>
-    <t>Safety validation for Stoic negative visualization practices. CRITICAL for vulnerable users (GAD‚â•15). Clinical + philosophical review required before launch. One-time pre-launch validation.</t>
-  </si>
-  <si>
     <t>Crisis Protocols (PHQ-9/GAD-7)</t>
   </si>
   <si>
@@ -284,39 +281,15 @@
     <t>Compliance &amp; Security</t>
   </si>
   <si>
-    <t>HIPAA Compliance Consultation (BAA-Free Validation)</t>
-  </si>
-  <si>
-    <t>ONE-TIME legal counsel confirmation that NO PHI transmitted, eliminating BAA requirements. Critical success factor unlocking $108K-326K savings over 5 years. Pre-launch.</t>
-  </si>
-  <si>
-    <t>Privacy Law Compliance (Initial Setup)</t>
-  </si>
-  <si>
-    <t>CCPA/VCDPA/GDPR privacy policy drafting, state-specific compliance review (CA/VA/CO), consent framework design. Required for App Store launch.</t>
-  </si>
-  <si>
     <t>Privacy Law Compliance (Ongoing)</t>
   </si>
   <si>
-    <t xml:space="preserve"> $1000-3000 </t>
-  </si>
-  <si>
     <t>Quarterly privacy policy reviews, state law updates monitoring, annual comprehensive review. Ongoing compliance maintenance.</t>
   </si>
   <si>
-    <t>Legal Counsel (Initial Setup)</t>
-  </si>
-  <si>
-    <t>Terms of Service drafting, Privacy Policy (mental health specific), Data Retention Policy. Required for App Store launch.</t>
-  </si>
-  <si>
     <t>Legal Counsel (Ongoing)</t>
   </si>
   <si>
-    <t xml:space="preserve"> $2000-5000 </t>
-  </si>
-  <si>
     <t>Quarterly reviews, ad-hoc consultations, regulatory change reviews. Hourly rate model more cost-effective than retainer for solo dev.</t>
   </si>
   <si>
@@ -347,24 +320,12 @@
     <t>NOT needed for consumer app. Annual certification cost if pursuing B2B/enterprise healthcare partnerships. Verify Supabase has SOC 2 Type II (no cost to Being).</t>
   </si>
   <si>
-    <t>App Store Privacy Compliance (Initial)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> $500-2000 </t>
-  </si>
-  <si>
-    <t>Privacy Nutrition Label (Apple), Data Safety Section (Google). Launch requirement. Primarily developer time (8-16 hours).</t>
-  </si>
-  <si>
     <t>App Store Privacy Compliance (Ongoing)</t>
   </si>
   <si>
     <t xml:space="preserve"> $300-1000 </t>
   </si>
   <si>
-    <t>Quarterly review for policy changes, updates for new app features. Developer time (2-4 hours/quarter). Ongoing compliance.</t>
-  </si>
-  <si>
     <t>User Consent Management System (Implementation)</t>
   </si>
   <si>
@@ -404,12 +365,6 @@
     <t>k-anonymity validation library, differential privacy implementation, PHI detection system. Tooling cost: $0-1000 (OSS libraries). Development time AI-accelerable. Quality assurance.</t>
   </si>
   <si>
-    <t>State Mental Health App Regulations (Research)</t>
-  </si>
-  <si>
-    <t>State-by-state regulatory analysis, mental health-specific app requirements (CA, NY, IL). Can phase by state of initial users.</t>
-  </si>
-  <si>
     <t>State Mental Health App Regulations (Monitoring)</t>
   </si>
   <si>
@@ -821,9 +776,6 @@
     <t xml:space="preserve"> $3000-5000 </t>
   </si>
   <si>
-    <t>y</t>
-  </si>
-  <si>
     <t xml:space="preserve"> $0-25 </t>
   </si>
   <si>
@@ -831,6 +783,18 @@
   </si>
   <si>
     <t>$0-1500</t>
+  </si>
+  <si>
+    <t>Pre-Launch Legal Package (Bundled)</t>
+  </si>
+  <si>
+    <t>Clinical safety review by licensed mental health professional (LMFT/psychologist) to assess psychological risk of negative visualization practices for vulnerable users (GAD≥15). Deliverable: Written safety assessment with recommendations. Legal review included in Pre-Launch Legal Package (separate row). Philosophical validation handled internally via classical texts + AI.</t>
+  </si>
+  <si>
+    <t>Quarterly legal review (2-4 hours) + developer time (2-4 hours) to update Privacy Nutrition Label and Data Safety. Section for policy changes and new features. Hourly rate model. Initial setup included in Pre-Launch Legal Package (separate row).</t>
+  </si>
+  <si>
+    <t>AI-assisted legal package: (1) AI drafts Privacy Policy (CCPA/VCDPA/GDPR compliant), Terms of Service, liability disclaimers, Premeditatio Malorum informed consent - $0 AI time; (2) Lawyer review of all AI-drafted docs - $500-800 (1-2 hrs); (3) HIPAA/BAA-free architecture consultation confirming no PHI transmission - $300-500 (30-60 min); (4) App Store privacy labels - DIY with AI guidance, $0. State mental health regs (CA/NY/IL) deferred to post-launch/scale phase. Requires lawyer with digital health/privacy experience but not full engagement. Savings vs traditional drafting: $3,000-4,500.</t>
   </si>
 </sst>
 </file>
@@ -1318,13 +1282,16 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
@@ -1699,26 +1666,47 @@
 </a:theme>
 </file>
 
+<file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
+<wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
+  <wetp:taskpane dockstate="right" visibility="0" width="350" row="0">
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+  </wetp:taskpane>
+</wetp:taskpanes>
+</file>
+
+<file path=xl/webextensions/webextension1.xml><?xml version="1.0" encoding="utf-8"?>
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{06A80BC8-04B3-A340-8064-DADDD190249A}">
+  <we:reference id="wa200009404" version="1.0.0.4" store="en-US" storeType="OMEX"/>
+  <we:alternateReferences>
+    <we:reference id="wa200009404" version="1.0.0.4" store="en-US" storeType="OMEX"/>
+  </we:alternateReferences>
+  <we:properties>
+    <we:property name="Office.AutoShowTaskpaneWithDocument" value="true"/>
+  </we:properties>
+  <we:bindings/>
+  <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+</we:webextension>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C78ECC95-93BA-E742-8CDF-F456D018CBC0}">
-  <dimension ref="A1:K105"/>
+  <dimension ref="A1:K101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F101" sqref="F101"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="29.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.6640625" customWidth="1"/>
+    <col min="2" max="2" width="34.1640625" customWidth="1"/>
     <col min="3" max="3" width="12.1640625" customWidth="1"/>
     <col min="4" max="4" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="10" customWidth="1"/>
     <col min="7" max="7" width="13.5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.33203125" customWidth="1"/>
     <col min="9" max="9" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="125.5" customWidth="1"/>
+    <col min="10" max="10" width="102.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
@@ -1790,7 +1778,7 @@
         <v>18</v>
       </c>
       <c r="K7" t="s">
-        <v>258</v>
+        <v>243</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
@@ -1849,7 +1837,7 @@
         <v>0</v>
       </c>
       <c r="H9" s="1">
-        <f t="shared" ref="H9:H69" si="0">IF(F9=0,G9,F9*12)</f>
+        <f>IF(F9=0,G9,F9*12)</f>
         <v>1188</v>
       </c>
       <c r="I9" t="s">
@@ -1882,7 +1870,7 @@
         <v>0</v>
       </c>
       <c r="H10" s="1">
-        <f t="shared" si="0"/>
+        <f>IF(F10=0,G10,F10*12)</f>
         <v>0</v>
       </c>
       <c r="I10" t="s">
@@ -1897,7 +1885,7 @@
         <v>19</v>
       </c>
       <c r="B11" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="C11" t="s">
         <v>21</v>
@@ -1906,23 +1894,23 @@
         <v>22</v>
       </c>
       <c r="E11" t="s">
-        <v>31</v>
-      </c>
-      <c r="F11" s="1">
-        <v>25</v>
+        <v>23</v>
+      </c>
+      <c r="F11" s="2">
+        <v>0</v>
       </c>
       <c r="G11" s="1">
         <v>0</v>
       </c>
       <c r="H11" s="1">
-        <f t="shared" si="0"/>
-        <v>300</v>
+        <f>IF(F11=0,G11,F11*12)</f>
+        <v>0</v>
       </c>
       <c r="I11" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J11" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
@@ -1930,7 +1918,7 @@
         <v>19</v>
       </c>
       <c r="B12" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="C12" t="s">
         <v>21</v>
@@ -1939,23 +1927,23 @@
         <v>22</v>
       </c>
       <c r="E12" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="F12" s="1">
-        <v>599</v>
+        <v>0</v>
       </c>
       <c r="G12" s="1">
         <v>0</v>
       </c>
       <c r="H12" s="1">
-        <f t="shared" si="0"/>
-        <v>7188</v>
+        <f>IF(F12=0,G12,F12*12)</f>
+        <v>0</v>
       </c>
       <c r="I12" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="J12" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
@@ -1963,32 +1951,32 @@
         <v>19</v>
       </c>
       <c r="B13" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="C13" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="D13" t="s">
         <v>22</v>
       </c>
       <c r="E13" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="F13" s="1">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="G13" s="1">
         <v>0</v>
       </c>
       <c r="H13" s="1">
-        <f t="shared" si="0"/>
-        <v>120</v>
+        <f>IF(F13=0,G13,F13*12)</f>
+        <v>0</v>
       </c>
       <c r="I13" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="J13" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
@@ -1996,7 +1984,7 @@
         <v>19</v>
       </c>
       <c r="B14" t="s">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="C14" t="s">
         <v>21</v>
@@ -2007,38 +1995,38 @@
       <c r="E14" t="s">
         <v>23</v>
       </c>
-      <c r="F14" s="2">
+      <c r="F14" s="1">
         <v>0</v>
       </c>
       <c r="G14" s="1">
         <v>0</v>
       </c>
       <c r="H14" s="1">
-        <f t="shared" si="0"/>
+        <f>IF(F14=0,G14,F14*12)</f>
         <v>0</v>
       </c>
       <c r="I14" t="s">
         <v>1</v>
       </c>
       <c r="J14" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>62</v>
       </c>
       <c r="B15" t="s">
-        <v>42</v>
+        <v>64</v>
       </c>
       <c r="C15" t="s">
         <v>21</v>
       </c>
       <c r="D15" t="s">
-        <v>22</v>
+        <v>65</v>
       </c>
       <c r="E15" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="F15" s="1">
         <v>0</v>
@@ -2047,61 +2035,61 @@
         <v>0</v>
       </c>
       <c r="H15" s="1">
-        <f t="shared" si="0"/>
+        <f>IF(F15=0,G15,F15*12)</f>
         <v>0</v>
       </c>
       <c r="I15" t="s">
         <v>1</v>
       </c>
       <c r="J15" t="s">
-        <v>44</v>
+        <v>66</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>62</v>
       </c>
       <c r="B16" t="s">
-        <v>45</v>
+        <v>69</v>
       </c>
       <c r="C16" t="s">
         <v>21</v>
       </c>
       <c r="D16" t="s">
-        <v>22</v>
+        <v>65</v>
       </c>
       <c r="E16" t="s">
-        <v>46</v>
+        <v>23</v>
       </c>
       <c r="F16" s="1">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="G16" s="1">
         <v>0</v>
       </c>
       <c r="H16" s="1">
-        <f t="shared" si="0"/>
-        <v>144</v>
+        <f>IF(F16=0,G16,F16*12)</f>
+        <v>0</v>
       </c>
       <c r="I16" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J16" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>62</v>
       </c>
       <c r="B17" t="s">
-        <v>48</v>
+        <v>74</v>
       </c>
       <c r="C17" t="s">
         <v>21</v>
       </c>
       <c r="D17" t="s">
-        <v>22</v>
+        <v>65</v>
       </c>
       <c r="E17" t="s">
         <v>23</v>
@@ -2110,31 +2098,31 @@
         <v>0</v>
       </c>
       <c r="G17" s="1">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="H17" s="1">
-        <f t="shared" si="0"/>
-        <v>35</v>
+        <f>IF(F17=0,G17,F17*12)</f>
+        <v>0</v>
       </c>
       <c r="I17" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="J17" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>19</v>
+        <v>62</v>
       </c>
       <c r="B18" t="s">
-        <v>50</v>
+        <v>78</v>
       </c>
       <c r="C18" t="s">
         <v>21</v>
       </c>
       <c r="D18" t="s">
-        <v>22</v>
+        <v>65</v>
       </c>
       <c r="E18" t="s">
         <v>23</v>
@@ -2146,121 +2134,121 @@
         <v>0</v>
       </c>
       <c r="H18" s="1">
-        <f t="shared" si="0"/>
+        <f>IF(F18=0,G18,F18*12)</f>
         <v>0</v>
       </c>
       <c r="I18" t="s">
         <v>1</v>
       </c>
       <c r="J18" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="177" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>19</v>
+        <v>80</v>
       </c>
       <c r="B19" t="s">
-        <v>52</v>
+        <v>249</v>
       </c>
       <c r="C19" t="s">
         <v>21</v>
       </c>
       <c r="D19" t="s">
-        <v>22</v>
+        <v>65</v>
       </c>
       <c r="E19" t="s">
-        <v>53</v>
+        <v>23</v>
       </c>
       <c r="F19" s="1">
         <v>0</v>
       </c>
       <c r="G19" s="1">
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="H19" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>IF(F19=0,G19,F19*12)</f>
+        <v>5000</v>
       </c>
       <c r="I19" t="s">
-        <v>3</v>
-      </c>
-      <c r="J19" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="J19" s="4" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>80</v>
       </c>
       <c r="B20" t="s">
-        <v>55</v>
+        <v>85</v>
       </c>
       <c r="C20" t="s">
         <v>21</v>
       </c>
       <c r="D20" t="s">
-        <v>22</v>
+        <v>65</v>
       </c>
       <c r="E20" t="s">
-        <v>56</v>
+        <v>23</v>
       </c>
       <c r="F20" s="1">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="G20" s="1">
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="H20" s="1">
-        <f t="shared" si="0"/>
-        <v>348</v>
+        <f>IF(F20=0,G20,F20*12)</f>
+        <v>5000</v>
       </c>
       <c r="I20" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J20" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>19</v>
+        <v>80</v>
       </c>
       <c r="B21" t="s">
-        <v>58</v>
+        <v>96</v>
       </c>
       <c r="C21" t="s">
         <v>21</v>
       </c>
       <c r="D21" t="s">
-        <v>22</v>
+        <v>65</v>
       </c>
       <c r="E21" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="F21" s="1">
-        <v>99</v>
+        <v>0</v>
       </c>
       <c r="G21" s="1">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="H21" s="1">
-        <f t="shared" si="0"/>
-        <v>1188</v>
+        <f>IF(F21=0,G21,F21*12)</f>
+        <v>1000</v>
       </c>
       <c r="I21" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="J21" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>19</v>
+        <v>111</v>
       </c>
       <c r="B22" t="s">
-        <v>60</v>
+        <v>117</v>
       </c>
       <c r="C22" t="s">
         <v>21</v>
@@ -2278,22 +2266,22 @@
         <v>0</v>
       </c>
       <c r="H22" s="1">
-        <f t="shared" si="0"/>
+        <f>IF(F22=0,G22,F22*12)</f>
         <v>0</v>
       </c>
       <c r="I22" t="s">
         <v>1</v>
       </c>
       <c r="J22" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>62</v>
+        <v>124</v>
       </c>
       <c r="B23" t="s">
-        <v>63</v>
+        <v>129</v>
       </c>
       <c r="C23" t="s">
         <v>21</v>
@@ -2308,31 +2296,31 @@
         <v>0</v>
       </c>
       <c r="G23" s="1">
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="H23" s="1">
-        <f t="shared" si="0"/>
-        <v>500</v>
+        <f>IF(F23=0,G23,F23*12)</f>
+        <v>0</v>
       </c>
       <c r="I23" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="J23" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>62</v>
+        <v>137</v>
       </c>
       <c r="B24" t="s">
-        <v>64</v>
+        <v>138</v>
       </c>
       <c r="C24" t="s">
         <v>21</v>
       </c>
       <c r="D24" t="s">
-        <v>65</v>
+        <v>22</v>
       </c>
       <c r="E24" t="s">
         <v>23</v>
@@ -2341,28 +2329,28 @@
         <v>0</v>
       </c>
       <c r="G24" s="1">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="H24" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>IF(F24=0,G24,F24*12)</f>
+        <v>1000</v>
       </c>
       <c r="I24" t="s">
         <v>1</v>
       </c>
       <c r="J24" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>62</v>
+        <v>137</v>
       </c>
       <c r="B25" t="s">
-        <v>67</v>
+        <v>142</v>
       </c>
       <c r="C25" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="D25" t="s">
         <v>22</v>
@@ -2370,65 +2358,65 @@
       <c r="E25" t="s">
         <v>23</v>
       </c>
-      <c r="F25" s="1">
-        <v>0</v>
+      <c r="F25" s="1" t="s">
+        <v>143</v>
       </c>
       <c r="G25" s="1">
         <v>0</v>
       </c>
-      <c r="H25" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
+      <c r="H25" s="1" t="e">
+        <f>IF(F25=0,G25,F25*12)</f>
+        <v>#VALUE!</v>
       </c>
       <c r="I25" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="J25" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>62</v>
+        <v>137</v>
       </c>
       <c r="B26" t="s">
-        <v>69</v>
+        <v>146</v>
       </c>
       <c r="C26" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="D26" t="s">
-        <v>65</v>
+        <v>22</v>
       </c>
       <c r="E26" t="s">
         <v>23</v>
       </c>
-      <c r="F26" s="1">
-        <v>0</v>
+      <c r="F26" s="1" t="s">
+        <v>143</v>
       </c>
       <c r="G26" s="1">
         <v>0</v>
       </c>
-      <c r="H26" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
+      <c r="H26" s="1" t="e">
+        <f>IF(F26=0,G26,F26*12)</f>
+        <v>#VALUE!</v>
       </c>
       <c r="I26" t="s">
         <v>1</v>
       </c>
       <c r="J26" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>62</v>
+        <v>137</v>
       </c>
       <c r="B27" t="s">
-        <v>71</v>
+        <v>151</v>
       </c>
       <c r="C27" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="D27" t="s">
         <v>22</v>
@@ -2443,94 +2431,91 @@
         <v>0</v>
       </c>
       <c r="H27" s="1">
-        <f t="shared" si="0"/>
+        <f>IF(F27=0,G27,F27*12)</f>
         <v>0</v>
       </c>
       <c r="I27" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="J27" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>62</v>
+        <v>137</v>
       </c>
       <c r="B28" t="s">
-        <v>73</v>
+        <v>153</v>
       </c>
       <c r="C28" t="s">
         <v>21</v>
       </c>
       <c r="D28" t="s">
-        <v>65</v>
+        <v>22</v>
       </c>
       <c r="E28" t="s">
         <v>23</v>
       </c>
       <c r="F28" s="1">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G28" s="1">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="H28" s="1">
-        <f t="shared" si="0"/>
-        <v>1000</v>
+        <f>IF(F28=0,G28,F28*12)</f>
+        <v>240</v>
       </c>
       <c r="I28" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="J28" t="s">
-        <v>74</v>
-      </c>
-      <c r="K28" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>62</v>
+        <v>137</v>
       </c>
       <c r="B29" t="s">
-        <v>75</v>
+        <v>161</v>
       </c>
       <c r="C29" t="s">
         <v>21</v>
       </c>
       <c r="D29" t="s">
-        <v>65</v>
+        <v>22</v>
       </c>
       <c r="E29" t="s">
         <v>23</v>
       </c>
       <c r="F29" s="1">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="G29" s="1">
         <v>0</v>
       </c>
       <c r="H29" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>IF(F29=0,G29,F29*12)</f>
+        <v>360</v>
       </c>
       <c r="I29" t="s">
         <v>1</v>
       </c>
       <c r="J29" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>62</v>
+        <v>137</v>
       </c>
       <c r="B30" t="s">
-        <v>77</v>
+        <v>164</v>
       </c>
       <c r="C30" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="D30" t="s">
         <v>22</v>
@@ -2542,31 +2527,32 @@
         <v>0</v>
       </c>
       <c r="G30" s="1">
-        <v>0</v>
+        <f>125+50</f>
+        <v>175</v>
       </c>
       <c r="H30" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>IF(F30=0,G30,F30*12)</f>
+        <v>175</v>
       </c>
       <c r="I30" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J30" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>62</v>
+        <v>137</v>
       </c>
       <c r="B31" t="s">
-        <v>79</v>
+        <v>166</v>
       </c>
       <c r="C31" t="s">
         <v>21</v>
       </c>
       <c r="D31" t="s">
-        <v>65</v>
+        <v>22</v>
       </c>
       <c r="E31" t="s">
         <v>23</v>
@@ -2575,25 +2561,25 @@
         <v>0</v>
       </c>
       <c r="G31" s="1">
-        <v>0</v>
+        <v>99</v>
       </c>
       <c r="H31" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>IF(F31=0,G31,F31*12)</f>
+        <v>99</v>
       </c>
       <c r="I31" t="s">
         <v>1</v>
       </c>
       <c r="J31" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>81</v>
+        <v>137</v>
       </c>
       <c r="B32" t="s">
-        <v>82</v>
+        <v>168</v>
       </c>
       <c r="C32" t="s">
         <v>21</v>
@@ -2608,25 +2594,25 @@
         <v>0</v>
       </c>
       <c r="G32" s="1">
-        <v>3000</v>
+        <v>25</v>
       </c>
       <c r="H32" s="1">
-        <f t="shared" si="0"/>
-        <v>3000</v>
+        <f>IF(F32=0,G32,F32*12)</f>
+        <v>25</v>
       </c>
       <c r="I32" t="s">
         <v>1</v>
       </c>
       <c r="J32" t="s">
-        <v>83</v>
+        <v>169</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>81</v>
+        <v>194</v>
       </c>
       <c r="B33" t="s">
-        <v>84</v>
+        <v>197</v>
       </c>
       <c r="C33" t="s">
         <v>21</v>
@@ -2641,31 +2627,28 @@
         <v>0</v>
       </c>
       <c r="G33" s="1">
-        <v>5000</v>
+        <v>0</v>
       </c>
       <c r="H33" s="1">
-        <f t="shared" si="0"/>
-        <v>5000</v>
+        <f>IF(F33=0,G33,F33*12)</f>
+        <v>0</v>
       </c>
       <c r="I33" t="s">
         <v>1</v>
       </c>
       <c r="J33" t="s">
-        <v>85</v>
-      </c>
-      <c r="K33" t="s">
-        <v>261</v>
+        <v>198</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>81</v>
+        <v>206</v>
       </c>
       <c r="B34" t="s">
-        <v>86</v>
+        <v>210</v>
       </c>
       <c r="C34" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="D34" t="s">
         <v>22</v>
@@ -2676,35 +2659,32 @@
       <c r="F34" s="1">
         <v>0</v>
       </c>
-      <c r="G34" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="H34" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> $1000-3000 </v>
+      <c r="G34" s="1">
+        <v>0</v>
+      </c>
+      <c r="H34" s="1">
+        <f>IF(F34=0,G34,F34*12)</f>
+        <v>0</v>
       </c>
       <c r="I34" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J34" t="s">
-        <v>88</v>
-      </c>
-      <c r="K34" s="1" t="s">
-        <v>261</v>
+        <v>211</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>81</v>
+        <v>206</v>
       </c>
       <c r="B35" t="s">
-        <v>89</v>
+        <v>212</v>
       </c>
       <c r="C35" t="s">
         <v>21</v>
       </c>
       <c r="D35" t="s">
-        <v>65</v>
+        <v>22</v>
       </c>
       <c r="E35" t="s">
         <v>23</v>
@@ -2713,28 +2693,28 @@
         <v>0</v>
       </c>
       <c r="G35" s="1">
-        <v>5000</v>
+        <v>0</v>
       </c>
       <c r="H35" s="1">
-        <f t="shared" si="0"/>
-        <v>5000</v>
+        <f>IF(F35=0,G35,F35*12)</f>
+        <v>0</v>
       </c>
       <c r="I35" t="s">
         <v>1</v>
       </c>
       <c r="J35" t="s">
-        <v>90</v>
+        <v>213</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>81</v>
+        <v>206</v>
       </c>
       <c r="B36" t="s">
-        <v>91</v>
+        <v>214</v>
       </c>
       <c r="C36" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="D36" t="s">
         <v>22</v>
@@ -2745,32 +2725,32 @@
       <c r="F36" s="1">
         <v>0</v>
       </c>
-      <c r="G36" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="H36" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> $2000-5000 </v>
+      <c r="G36" s="1">
+        <v>0</v>
+      </c>
+      <c r="H36" s="1">
+        <f>IF(F36=0,G36,F36*12)</f>
+        <v>0</v>
       </c>
       <c r="I36" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J36" t="s">
-        <v>93</v>
+        <v>215</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>81</v>
+        <v>220</v>
       </c>
       <c r="B37" t="s">
-        <v>94</v>
+        <v>221</v>
       </c>
       <c r="C37" t="s">
         <v>21</v>
       </c>
       <c r="D37" t="s">
-        <v>65</v>
+        <v>22</v>
       </c>
       <c r="E37" t="s">
         <v>23</v>
@@ -2779,58 +2759,58 @@
         <v>0</v>
       </c>
       <c r="G37" s="1">
-        <v>5000</v>
+        <v>0</v>
       </c>
       <c r="H37" s="1">
-        <f t="shared" si="0"/>
-        <v>5000</v>
+        <f>IF(F37=0,G37,F37*12)</f>
+        <v>0</v>
       </c>
       <c r="I37" t="s">
         <v>1</v>
       </c>
       <c r="J37" t="s">
-        <v>95</v>
+        <v>222</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>81</v>
+        <v>19</v>
       </c>
       <c r="B38" t="s">
-        <v>96</v>
+        <v>30</v>
       </c>
       <c r="C38" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="D38" t="s">
         <v>22</v>
       </c>
       <c r="E38" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="F38" s="1">
-        <v>0</v>
-      </c>
-      <c r="G38" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="H38" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> $3000-5000 </v>
+        <v>25</v>
+      </c>
+      <c r="G38" s="1">
+        <v>0</v>
+      </c>
+      <c r="H38" s="1">
+        <f>IF(F38=0,G38,F38*12)</f>
+        <v>300</v>
       </c>
       <c r="I38" t="s">
         <v>3</v>
       </c>
       <c r="J38" t="s">
-        <v>97</v>
+        <v>32</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>81</v>
+        <v>19</v>
       </c>
       <c r="B39" t="s">
-        <v>98</v>
+        <v>45</v>
       </c>
       <c r="C39" t="s">
         <v>21</v>
@@ -2839,31 +2819,31 @@
         <v>22</v>
       </c>
       <c r="E39" t="s">
-        <v>23</v>
+        <v>46</v>
       </c>
       <c r="F39" s="1">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="G39" s="1">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="H39" s="1">
-        <f t="shared" si="0"/>
-        <v>1000</v>
+        <f>IF(F39=0,G39,F39*12)</f>
+        <v>144</v>
       </c>
       <c r="I39" t="s">
         <v>3</v>
       </c>
       <c r="J39" t="s">
-        <v>99</v>
+        <v>47</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>81</v>
+        <v>19</v>
       </c>
       <c r="B40" t="s">
-        <v>100</v>
+        <v>52</v>
       </c>
       <c r="C40" t="s">
         <v>21</v>
@@ -2872,67 +2852,64 @@
         <v>22</v>
       </c>
       <c r="E40" t="s">
-        <v>23</v>
+        <v>53</v>
       </c>
       <c r="F40" s="1">
         <v>0</v>
       </c>
-      <c r="G40" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="H40" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> $15000-50000 </v>
+      <c r="G40" s="1">
+        <v>0</v>
+      </c>
+      <c r="H40" s="1">
+        <f>IF(F40=0,G40,F40*12)</f>
+        <v>0</v>
       </c>
       <c r="I40" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="J40" t="s">
-        <v>102</v>
+        <v>54</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>81</v>
+        <v>19</v>
       </c>
       <c r="B41" t="s">
-        <v>103</v>
+        <v>55</v>
       </c>
       <c r="C41" t="s">
         <v>21</v>
       </c>
       <c r="D41" t="s">
-        <v>65</v>
+        <v>22</v>
       </c>
       <c r="E41" t="s">
-        <v>23</v>
+        <v>56</v>
       </c>
       <c r="F41" s="1">
-        <v>0</v>
-      </c>
-      <c r="G41" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="H41" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> $500-2000 </v>
+        <v>29</v>
+      </c>
+      <c r="G41" s="1">
+        <v>0</v>
+      </c>
+      <c r="H41" s="1">
+        <f>IF(F41=0,G41,F41*12)</f>
+        <v>348</v>
       </c>
       <c r="I41" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J41" t="s">
-        <v>105</v>
-      </c>
-      <c r="K41" s="1" t="s">
-        <v>261</v>
+        <v>57</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>81</v>
+        <v>62</v>
       </c>
       <c r="B42" t="s">
-        <v>106</v>
+        <v>76</v>
       </c>
       <c r="C42" t="s">
         <v>37</v>
@@ -2946,35 +2923,32 @@
       <c r="F42" s="1">
         <v>0</v>
       </c>
-      <c r="G42" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="H42" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> $300-1000 </v>
+      <c r="G42" s="1">
+        <v>0</v>
+      </c>
+      <c r="H42" s="1">
+        <f>IF(F42=0,G42,F42*12)</f>
+        <v>0</v>
       </c>
       <c r="I42" t="s">
         <v>3</v>
       </c>
       <c r="J42" t="s">
-        <v>108</v>
-      </c>
-      <c r="K42" s="1" t="s">
-        <v>261</v>
+        <v>77</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
+        <v>80</v>
+      </c>
+      <c r="B43" t="s">
         <v>81</v>
       </c>
-      <c r="B43" t="s">
-        <v>109</v>
-      </c>
       <c r="C43" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="D43" t="s">
-        <v>65</v>
+        <v>22</v>
       </c>
       <c r="E43" t="s">
         <v>23</v>
@@ -2986,22 +2960,23 @@
         <v>1000</v>
       </c>
       <c r="H43" s="1">
-        <f t="shared" si="0"/>
+        <f>IF(F43=0,G43,F43*12)</f>
         <v>1000</v>
       </c>
       <c r="I43" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J43" t="s">
-        <v>110</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="K43" s="1"/>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B44" t="s">
-        <v>111</v>
+        <v>83</v>
       </c>
       <c r="C44" t="s">
         <v>37</v>
@@ -3015,32 +2990,32 @@
       <c r="F44" s="1">
         <v>0</v>
       </c>
-      <c r="G44" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="H44" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> $200-500 </v>
+      <c r="G44" s="1">
+        <v>2000</v>
+      </c>
+      <c r="H44" s="1">
+        <f>IF(F44=0,G44,F44*12)</f>
+        <v>2000</v>
       </c>
       <c r="I44" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="J44" t="s">
-        <v>113</v>
+        <v>84</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B45" t="s">
-        <v>114</v>
+        <v>87</v>
       </c>
       <c r="C45" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="D45" t="s">
-        <v>65</v>
+        <v>22</v>
       </c>
       <c r="E45" t="s">
         <v>23</v>
@@ -3048,29 +3023,29 @@
       <c r="F45" s="1">
         <v>0</v>
       </c>
-      <c r="G45" s="1">
-        <v>1000</v>
-      </c>
-      <c r="H45" s="1">
-        <f t="shared" si="0"/>
-        <v>1000</v>
+      <c r="G45" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="H45" s="1" t="str">
+        <f>IF(F45=0,G45,F45*12)</f>
+        <v xml:space="preserve"> $3000-5000 </v>
       </c>
       <c r="I45" t="s">
         <v>3</v>
       </c>
       <c r="J45" t="s">
-        <v>115</v>
+        <v>88</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B46" t="s">
-        <v>116</v>
+        <v>89</v>
       </c>
       <c r="C46" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="D46" t="s">
         <v>22</v>
@@ -3081,32 +3056,32 @@
       <c r="F46" s="1">
         <v>0</v>
       </c>
-      <c r="G46" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="H46" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> $500-1000 </v>
+      <c r="G46" s="1">
+        <v>1000</v>
+      </c>
+      <c r="H46" s="1">
+        <f>IF(F46=0,G46,F46*12)</f>
+        <v>1000</v>
       </c>
       <c r="I46" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="J46" t="s">
-        <v>118</v>
+        <v>90</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B47" t="s">
-        <v>119</v>
+        <v>94</v>
       </c>
       <c r="C47" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="D47" t="s">
-        <v>65</v>
+        <v>22</v>
       </c>
       <c r="E47" t="s">
         <v>23</v>
@@ -3115,25 +3090,26 @@
         <v>0</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>120</v>
+        <v>95</v>
       </c>
       <c r="H47" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> $0-1000 </v>
+        <f>IF(F47=0,G47,F47*12)</f>
+        <v xml:space="preserve"> $300-1000 </v>
       </c>
       <c r="I47" t="s">
         <v>3</v>
       </c>
       <c r="J47" t="s">
-        <v>121</v>
-      </c>
+        <v>251</v>
+      </c>
+      <c r="K47" s="1"/>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B48" t="s">
-        <v>122</v>
+        <v>101</v>
       </c>
       <c r="C48" t="s">
         <v>21</v>
@@ -3147,35 +3123,32 @@
       <c r="F48" s="1">
         <v>0</v>
       </c>
-      <c r="G48" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="H48" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> $1000-3000 </v>
+      <c r="G48" s="1">
+        <v>1000</v>
+      </c>
+      <c r="H48" s="1">
+        <f>IF(F48=0,G48,F48*12)</f>
+        <v>1000</v>
       </c>
       <c r="I48" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="J48" t="s">
-        <v>123</v>
-      </c>
-      <c r="K48" s="1" t="s">
-        <v>261</v>
+        <v>102</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B49" t="s">
-        <v>124</v>
+        <v>106</v>
       </c>
       <c r="C49" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="D49" t="s">
-        <v>22</v>
+        <v>65</v>
       </c>
       <c r="E49" t="s">
         <v>23</v>
@@ -3184,91 +3157,91 @@
         <v>0</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="H49" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> $500-1500 </v>
+        <f>IF(F49=0,G49,F49*12)</f>
+        <v xml:space="preserve"> $0-1000 </v>
       </c>
       <c r="I49" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="J49" t="s">
-        <v>125</v>
+        <v>108</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>126</v>
+        <v>137</v>
       </c>
       <c r="B50" t="s">
-        <v>127</v>
+        <v>140</v>
       </c>
       <c r="C50" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="D50" t="s">
         <v>22</v>
       </c>
       <c r="E50" t="s">
-        <v>128</v>
+        <v>23</v>
       </c>
       <c r="F50" s="1">
-        <v>49</v>
-      </c>
-      <c r="G50" s="1">
-        <v>0</v>
-      </c>
-      <c r="H50" s="1">
-        <f t="shared" si="0"/>
-        <v>588</v>
+        <v>0</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="H50" s="1" t="str">
+        <f>IF(F50=0,G50,F50*12)</f>
+        <v>$0-1500</v>
       </c>
       <c r="I50" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="J50" t="s">
-        <v>129</v>
+        <v>141</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>126</v>
+        <v>137</v>
       </c>
       <c r="B51" t="s">
-        <v>130</v>
+        <v>155</v>
       </c>
       <c r="C51" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="D51" t="s">
         <v>22</v>
       </c>
       <c r="E51" t="s">
-        <v>128</v>
+        <v>23</v>
       </c>
       <c r="F51" s="1">
         <v>0</v>
       </c>
       <c r="G51" s="1">
-        <v>0</v>
+        <v>1500</v>
       </c>
       <c r="H51" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>IF(F51=0,G51,F51*12)</f>
+        <v>1500</v>
       </c>
       <c r="I51" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="J51" t="s">
-        <v>131</v>
+        <v>156</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>126</v>
+        <v>137</v>
       </c>
       <c r="B52" t="s">
-        <v>132</v>
+        <v>175</v>
       </c>
       <c r="C52" t="s">
         <v>21</v>
@@ -3279,62 +3252,62 @@
       <c r="E52" t="s">
         <v>23</v>
       </c>
-      <c r="F52" s="1">
-        <v>0</v>
-      </c>
-      <c r="G52" s="1">
-        <v>0</v>
+      <c r="F52" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>144</v>
       </c>
       <c r="H52" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>IF(F52=0,G52,F52*12)</f>
+        <v>1.2000000000000002</v>
       </c>
       <c r="I52" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J52" t="s">
-        <v>133</v>
+        <v>176</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>126</v>
+        <v>137</v>
       </c>
       <c r="B53" t="s">
-        <v>134</v>
+        <v>177</v>
       </c>
       <c r="C53" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="D53" t="s">
         <v>22</v>
       </c>
       <c r="E53" t="s">
-        <v>135</v>
-      </c>
-      <c r="F53" s="1">
-        <v>15</v>
-      </c>
-      <c r="G53" s="1">
-        <v>0</v>
+        <v>23</v>
+      </c>
+      <c r="F53" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>144</v>
       </c>
       <c r="H53" s="1">
-        <f t="shared" si="0"/>
-        <v>180</v>
+        <f>IF(F53=0,G53,F53*12)</f>
+        <v>1.2000000000000002</v>
       </c>
       <c r="I53" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="J53" t="s">
-        <v>136</v>
+        <v>178</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>126</v>
+        <v>179</v>
       </c>
       <c r="B54" t="s">
-        <v>137</v>
+        <v>185</v>
       </c>
       <c r="C54" t="s">
         <v>21</v>
@@ -3352,22 +3325,22 @@
         <v>0</v>
       </c>
       <c r="H54" s="1">
-        <f t="shared" si="0"/>
+        <f>IF(F54=0,G54,F54*12)</f>
         <v>0</v>
       </c>
       <c r="I54" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="J54" t="s">
-        <v>138</v>
+        <v>186</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>139</v>
+        <v>179</v>
       </c>
       <c r="B55" t="s">
-        <v>140</v>
+        <v>187</v>
       </c>
       <c r="C55" t="s">
         <v>21</v>
@@ -3379,28 +3352,29 @@
         <v>23</v>
       </c>
       <c r="F55" s="1">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G55" s="1">
         <v>0</v>
       </c>
       <c r="H55" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>IF(F55=0,G55,F55*12)</f>
+        <v>60</v>
       </c>
       <c r="I55" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="J55" t="s">
-        <v>141</v>
-      </c>
+        <v>188</v>
+      </c>
+      <c r="K55" s="1"/>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>139</v>
+        <v>194</v>
       </c>
       <c r="B56" t="s">
-        <v>142</v>
+        <v>199</v>
       </c>
       <c r="C56" t="s">
         <v>37</v>
@@ -3418,28 +3392,28 @@
         <v>0</v>
       </c>
       <c r="H56" s="1">
-        <f t="shared" si="0"/>
+        <f>IF(F56=0,G56,F56*12)</f>
         <v>0</v>
       </c>
       <c r="I56" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="J56" t="s">
-        <v>143</v>
+        <v>200</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>139</v>
+        <v>194</v>
       </c>
       <c r="B57" t="s">
-        <v>144</v>
+        <v>204</v>
       </c>
       <c r="C57" t="s">
         <v>21</v>
       </c>
       <c r="D57" t="s">
-        <v>22</v>
+        <v>65</v>
       </c>
       <c r="E57" t="s">
         <v>23</v>
@@ -3447,32 +3421,32 @@
       <c r="F57" s="1">
         <v>0</v>
       </c>
-      <c r="G57" s="1">
-        <v>0</v>
-      </c>
-      <c r="H57" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
+      <c r="G57" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="H57" s="1" t="str">
+        <f>IF(F57=0,G57,F57*12)</f>
+        <v xml:space="preserve"> $500-1000 </v>
       </c>
       <c r="I57" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J57" t="s">
-        <v>145</v>
+        <v>205</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>139</v>
+        <v>206</v>
       </c>
       <c r="B58" t="s">
-        <v>146</v>
+        <v>207</v>
       </c>
       <c r="C58" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="D58" t="s">
-        <v>22</v>
+        <v>65</v>
       </c>
       <c r="E58" t="s">
         <v>23</v>
@@ -3480,59 +3454,59 @@
       <c r="F58" s="1">
         <v>0</v>
       </c>
-      <c r="G58" s="1">
-        <v>0</v>
-      </c>
-      <c r="H58" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
+      <c r="G58" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="H58" s="1" t="str">
+        <f>IF(F58=0,G58,F58*12)</f>
+        <v xml:space="preserve"> $1500-2000 </v>
       </c>
       <c r="I58" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="J58" t="s">
-        <v>147</v>
+        <v>209</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>139</v>
+        <v>19</v>
       </c>
       <c r="B59" t="s">
-        <v>148</v>
+        <v>33</v>
       </c>
       <c r="C59" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="D59" t="s">
         <v>22</v>
       </c>
       <c r="E59" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="F59" s="1">
-        <v>0</v>
+        <v>599</v>
       </c>
       <c r="G59" s="1">
         <v>0</v>
       </c>
       <c r="H59" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>IF(F59=0,G59,F59*12)</f>
+        <v>7188</v>
       </c>
       <c r="I59" t="s">
         <v>7</v>
       </c>
       <c r="J59" t="s">
-        <v>149</v>
+        <v>35</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>139</v>
+        <v>62</v>
       </c>
       <c r="B60" t="s">
-        <v>150</v>
+        <v>63</v>
       </c>
       <c r="C60" t="s">
         <v>21</v>
@@ -3544,28 +3518,28 @@
         <v>23</v>
       </c>
       <c r="F60" s="1">
+        <v>0</v>
+      </c>
+      <c r="G60" s="1">
         <v>500</v>
       </c>
-      <c r="G60" s="1">
-        <v>0</v>
-      </c>
       <c r="H60" s="1">
-        <f t="shared" si="0"/>
-        <v>6000</v>
+        <f>IF(F60=0,G60,F60*12)</f>
+        <v>500</v>
       </c>
       <c r="I60" t="s">
         <v>7</v>
       </c>
       <c r="J60" t="s">
-        <v>151</v>
+        <v>242</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>152</v>
+        <v>62</v>
       </c>
       <c r="B61" t="s">
-        <v>153</v>
+        <v>67</v>
       </c>
       <c r="C61" t="s">
         <v>21</v>
@@ -3580,31 +3554,28 @@
         <v>0</v>
       </c>
       <c r="G61" s="1">
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="H61" s="1">
-        <f t="shared" si="0"/>
-        <v>500</v>
+        <f>IF(F61=0,G61,F61*12)</f>
+        <v>0</v>
       </c>
       <c r="I61" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J61" t="s">
-        <v>154</v>
-      </c>
-      <c r="K61" t="s">
-        <v>261</v>
+        <v>68</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>152</v>
+        <v>80</v>
       </c>
       <c r="B62" t="s">
-        <v>155</v>
+        <v>91</v>
       </c>
       <c r="C62" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="D62" t="s">
         <v>22</v>
@@ -3616,58 +3587,58 @@
         <v>0</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>264</v>
+        <v>92</v>
       </c>
       <c r="H62" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>$0-1500</v>
+        <f>IF(F62=0,G62,F62*12)</f>
+        <v xml:space="preserve"> $15000-50000 </v>
       </c>
       <c r="I62" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="J62" t="s">
-        <v>156</v>
+        <v>93</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>152</v>
+        <v>111</v>
       </c>
       <c r="B63" t="s">
-        <v>157</v>
+        <v>122</v>
       </c>
       <c r="C63" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="D63" t="s">
-        <v>22</v>
+        <v>65</v>
       </c>
       <c r="E63" t="s">
         <v>23</v>
       </c>
-      <c r="F63" s="1" t="s">
-        <v>158</v>
+      <c r="F63" s="1">
+        <v>0</v>
       </c>
       <c r="G63" s="1">
         <v>0</v>
       </c>
-      <c r="H63" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+      <c r="H63" s="1">
+        <f>IF(F63=0,G63,F63*12)</f>
+        <v>0</v>
       </c>
       <c r="I63" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J63" t="s">
-        <v>160</v>
+        <v>123</v>
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>152</v>
+        <v>124</v>
       </c>
       <c r="B64" t="s">
-        <v>161</v>
+        <v>127</v>
       </c>
       <c r="C64" t="s">
         <v>37</v>
@@ -3678,29 +3649,29 @@
       <c r="E64" t="s">
         <v>23</v>
       </c>
-      <c r="F64" s="1" t="s">
-        <v>158</v>
+      <c r="F64" s="1">
+        <v>0</v>
       </c>
       <c r="G64" s="1">
         <v>0</v>
       </c>
-      <c r="H64" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+      <c r="H64" s="1">
+        <f>IF(F64=0,G64,F64*12)</f>
+        <v>0</v>
       </c>
       <c r="I64" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J64" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>152</v>
+        <v>124</v>
       </c>
       <c r="B65" t="s">
-        <v>163</v>
+        <v>131</v>
       </c>
       <c r="C65" t="s">
         <v>37</v>
@@ -3711,32 +3682,32 @@
       <c r="E65" t="s">
         <v>23</v>
       </c>
-      <c r="F65" s="1" t="s">
-        <v>164</v>
+      <c r="F65" s="1">
+        <v>0</v>
       </c>
       <c r="G65" s="1">
         <v>0</v>
       </c>
-      <c r="H65" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+      <c r="H65" s="1">
+        <f>IF(F65=0,G65,F65*12)</f>
+        <v>0</v>
       </c>
       <c r="I65" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="J65" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>152</v>
+        <v>124</v>
       </c>
       <c r="B66" t="s">
-        <v>166</v>
+        <v>133</v>
       </c>
       <c r="C66" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="D66" t="s">
         <v>22</v>
@@ -3751,22 +3722,22 @@
         <v>0</v>
       </c>
       <c r="H66" s="1">
-        <f t="shared" si="0"/>
+        <f>IF(F66=0,G66,F66*12)</f>
         <v>0</v>
       </c>
       <c r="I66" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J66" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>152</v>
+        <v>124</v>
       </c>
       <c r="B67" t="s">
-        <v>168</v>
+        <v>135</v>
       </c>
       <c r="C67" t="s">
         <v>21</v>
@@ -3778,28 +3749,28 @@
         <v>23</v>
       </c>
       <c r="F67" s="1">
-        <v>20</v>
+        <v>500</v>
       </c>
       <c r="G67" s="1">
         <v>0</v>
       </c>
       <c r="H67" s="1">
-        <f t="shared" si="0"/>
-        <v>240</v>
+        <f>IF(F67=0,G67,F67*12)</f>
+        <v>6000</v>
       </c>
       <c r="I67" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J67" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>152</v>
+        <v>137</v>
       </c>
       <c r="B68" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="C68" t="s">
         <v>21</v>
@@ -3814,31 +3785,31 @@
         <v>0</v>
       </c>
       <c r="G68" s="1">
-        <v>1500</v>
+        <v>500</v>
       </c>
       <c r="H68" s="1">
-        <f t="shared" si="0"/>
-        <v>1500</v>
+        <f>IF(F68=0,G68,F68*12)</f>
+        <v>500</v>
       </c>
       <c r="I68" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="J68" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>152</v>
+        <v>179</v>
       </c>
       <c r="B69" t="s">
-        <v>172</v>
+        <v>189</v>
       </c>
       <c r="C69" t="s">
         <v>21</v>
       </c>
       <c r="D69" t="s">
-        <v>22</v>
+        <v>65</v>
       </c>
       <c r="E69" t="s">
         <v>23</v>
@@ -3847,25 +3818,25 @@
         <v>0</v>
       </c>
       <c r="G69" s="1">
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="H69" s="1">
-        <f t="shared" si="0"/>
-        <v>1500</v>
+        <f>IF(F69=0,G69,F69*12)</f>
+        <v>1000</v>
       </c>
       <c r="I69" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="J69" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>152</v>
+        <v>194</v>
       </c>
       <c r="B70" t="s">
-        <v>174</v>
+        <v>195</v>
       </c>
       <c r="C70" t="s">
         <v>21</v>
@@ -3877,61 +3848,61 @@
         <v>23</v>
       </c>
       <c r="F70" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G70" s="1">
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="H70" s="1">
-        <f t="shared" ref="H70:H105" si="1">IF(F70=0,G70,F70*12)</f>
-        <v>500</v>
+        <f>IF(F70=0,G70,F70*12)</f>
+        <v>120</v>
       </c>
       <c r="I70" t="s">
         <v>7</v>
       </c>
       <c r="J70" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>152</v>
+        <v>220</v>
       </c>
       <c r="B71" t="s">
-        <v>176</v>
+        <v>223</v>
       </c>
       <c r="C71" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="D71" t="s">
         <v>22</v>
       </c>
       <c r="E71" t="s">
-        <v>23</v>
+        <v>224</v>
       </c>
       <c r="F71" s="1">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="G71" s="1">
         <v>0</v>
       </c>
       <c r="H71" s="1">
-        <f t="shared" si="1"/>
-        <v>360</v>
+        <f>IF(F71=0,G71,F71*12)</f>
+        <v>0</v>
       </c>
       <c r="I71" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J71" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>152</v>
+        <v>220</v>
       </c>
       <c r="B72" t="s">
-        <v>177</v>
+        <v>226</v>
       </c>
       <c r="C72" t="s">
         <v>37</v>
@@ -3942,63 +3913,62 @@
       <c r="E72" t="s">
         <v>23</v>
       </c>
-      <c r="F72" s="1" t="s">
-        <v>262</v>
+      <c r="F72" s="1">
+        <v>0</v>
       </c>
       <c r="G72" s="1">
         <v>0</v>
       </c>
-      <c r="H72" s="1" t="e">
-        <f t="shared" si="1"/>
-        <v>#VALUE!</v>
+      <c r="H72" s="1">
+        <f>IF(F72=0,G72,F72*12)</f>
+        <v>0</v>
       </c>
       <c r="I72" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="J72" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>152</v>
+        <v>220</v>
       </c>
       <c r="B73" t="s">
-        <v>179</v>
+        <v>228</v>
       </c>
       <c r="C73" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="D73" t="s">
         <v>22</v>
       </c>
       <c r="E73" t="s">
-        <v>23</v>
+        <v>229</v>
       </c>
       <c r="F73" s="1">
         <v>0</v>
       </c>
       <c r="G73" s="1">
-        <f>125+50</f>
-        <v>175</v>
+        <v>0</v>
       </c>
       <c r="H73" s="1">
-        <f t="shared" si="1"/>
-        <v>175</v>
+        <f>IF(F73=0,G73,F73*12)</f>
+        <v>0</v>
       </c>
       <c r="I73" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J73" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>152</v>
+        <v>231</v>
       </c>
       <c r="B74" t="s">
-        <v>181</v>
+        <v>232</v>
       </c>
       <c r="C74" t="s">
         <v>21</v>
@@ -4013,31 +3983,31 @@
         <v>0</v>
       </c>
       <c r="G74" s="1">
-        <v>99</v>
+        <v>2000</v>
       </c>
       <c r="H74" s="1">
-        <f t="shared" si="1"/>
-        <v>99</v>
+        <f>IF(F74=0,G74,F74*12)</f>
+        <v>2000</v>
       </c>
       <c r="I74" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J74" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>152</v>
+        <v>236</v>
       </c>
       <c r="B75" t="s">
-        <v>183</v>
+        <v>237</v>
       </c>
       <c r="C75" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="D75" t="s">
-        <v>65</v>
+        <v>22</v>
       </c>
       <c r="E75" t="s">
         <v>23</v>
@@ -4046,25 +4016,25 @@
         <v>0</v>
       </c>
       <c r="G75" s="1">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="H75" s="1">
-        <f t="shared" si="1"/>
-        <v>25</v>
+        <f>IF(F75=0,G75,F75*12)</f>
+        <v>0</v>
       </c>
       <c r="I75" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J75" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>152</v>
+        <v>236</v>
       </c>
       <c r="B76" t="s">
-        <v>185</v>
+        <v>239</v>
       </c>
       <c r="C76" t="s">
         <v>21</v>
@@ -4076,26 +4046,28 @@
         <v>23</v>
       </c>
       <c r="F76" s="1">
-        <v>50</v>
-      </c>
-      <c r="G76" s="1"/>
+        <v>0</v>
+      </c>
+      <c r="G76" s="1">
+        <v>200</v>
+      </c>
       <c r="H76" s="1">
-        <f t="shared" si="1"/>
-        <v>600</v>
+        <f>IF(F76=0,G76,F76*12)</f>
+        <v>200</v>
       </c>
       <c r="I76" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="J76" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>152</v>
+        <v>19</v>
       </c>
       <c r="B77" t="s">
-        <v>187</v>
+        <v>36</v>
       </c>
       <c r="C77" t="s">
         <v>37</v>
@@ -4104,31 +4076,31 @@
         <v>22</v>
       </c>
       <c r="E77" t="s">
-        <v>23</v>
-      </c>
-      <c r="F77" s="1" t="s">
-        <v>188</v>
+        <v>38</v>
+      </c>
+      <c r="F77" s="1">
+        <v>10</v>
       </c>
       <c r="G77" s="1">
         <v>0</v>
       </c>
-      <c r="H77" s="1" t="e">
-        <f t="shared" si="1"/>
-        <v>#VALUE!</v>
+      <c r="H77" s="1">
+        <f>IF(F77=0,G77,F77*12)</f>
+        <v>120</v>
       </c>
       <c r="I77" t="s">
         <v>5</v>
       </c>
       <c r="J77" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>152</v>
+        <v>19</v>
       </c>
       <c r="B78" t="s">
-        <v>190</v>
+        <v>48</v>
       </c>
       <c r="C78" t="s">
         <v>21</v>
@@ -4139,98 +4111,95 @@
       <c r="E78" t="s">
         <v>23</v>
       </c>
-      <c r="F78" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="G78" s="1" t="s">
-        <v>159</v>
+      <c r="F78" s="1">
+        <v>0</v>
+      </c>
+      <c r="G78" s="1">
+        <v>35</v>
       </c>
       <c r="H78" s="1">
-        <f t="shared" si="1"/>
-        <v>1.2000000000000002</v>
+        <f>IF(F78=0,G78,F78*12)</f>
+        <v>35</v>
       </c>
       <c r="I78" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="J78" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>152</v>
+        <v>19</v>
       </c>
       <c r="B79" t="s">
-        <v>192</v>
+        <v>58</v>
       </c>
       <c r="C79" t="s">
+        <v>21</v>
+      </c>
+      <c r="D79" t="s">
+        <v>22</v>
+      </c>
+      <c r="E79" t="s">
+        <v>31</v>
+      </c>
+      <c r="F79" s="1">
+        <v>99</v>
+      </c>
+      <c r="G79" s="1">
+        <v>0</v>
+      </c>
+      <c r="H79" s="1">
+        <f>IF(F79=0,G79,F79*12)</f>
+        <v>1188</v>
+      </c>
+      <c r="I79" t="s">
+        <v>5</v>
+      </c>
+      <c r="J79" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>62</v>
+      </c>
+      <c r="B80" t="s">
+        <v>71</v>
+      </c>
+      <c r="C80" t="s">
         <v>37</v>
       </c>
-      <c r="D79" t="s">
-        <v>22</v>
-      </c>
-      <c r="E79" t="s">
-        <v>23</v>
-      </c>
-      <c r="F79" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="G79" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="H79" s="1">
-        <f t="shared" si="1"/>
-        <v>1.2000000000000002</v>
-      </c>
-      <c r="I79" t="s">
-        <v>3</v>
-      </c>
-      <c r="J79" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A80" t="s">
-        <v>194</v>
-      </c>
-      <c r="B80" t="s">
-        <v>195</v>
-      </c>
-      <c r="C80" t="s">
-        <v>21</v>
-      </c>
       <c r="D80" t="s">
         <v>22</v>
       </c>
       <c r="E80" t="s">
         <v>23</v>
       </c>
-      <c r="F80" s="1" t="s">
-        <v>196</v>
+      <c r="F80" s="1">
+        <v>0</v>
       </c>
       <c r="G80" s="1">
         <v>0</v>
       </c>
-      <c r="H80" s="1" t="e">
-        <f t="shared" si="1"/>
-        <v>#VALUE!</v>
+      <c r="H80" s="1">
+        <f>IF(F80=0,G80,F80*12)</f>
+        <v>0</v>
       </c>
       <c r="I80" t="s">
         <v>5</v>
       </c>
       <c r="J80" t="s">
-        <v>197</v>
-      </c>
-      <c r="K80" s="1" t="s">
-        <v>261</v>
+        <v>72</v>
       </c>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>194</v>
+        <v>62</v>
       </c>
       <c r="B81" t="s">
-        <v>198</v>
+        <v>73</v>
       </c>
       <c r="C81" t="s">
         <v>21</v>
@@ -4245,31 +4214,34 @@
         <v>0</v>
       </c>
       <c r="G81" s="1">
-        <v>0</v>
+        <v>400</v>
       </c>
       <c r="H81" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>IF(F81=0,G81,F81*12)</f>
+        <v>400</v>
       </c>
       <c r="I81" t="s">
         <v>5</v>
       </c>
       <c r="J81" t="s">
-        <v>199</v>
+        <v>250</v>
+      </c>
+      <c r="K81" t="s">
+        <v>244</v>
       </c>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>194</v>
+        <v>80</v>
       </c>
       <c r="B82" t="s">
-        <v>200</v>
+        <v>98</v>
       </c>
       <c r="C82" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="D82" t="s">
-        <v>65</v>
+        <v>22</v>
       </c>
       <c r="E82" t="s">
         <v>23</v>
@@ -4277,68 +4249,65 @@
       <c r="F82" s="1">
         <v>0</v>
       </c>
-      <c r="G82" s="1">
-        <v>0</v>
-      </c>
-      <c r="H82" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="G82" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="H82" s="1" t="str">
+        <f>IF(F82=0,G82,F82*12)</f>
+        <v xml:space="preserve"> $200-500 </v>
       </c>
       <c r="I82" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="J82" t="s">
-        <v>201</v>
+        <v>100</v>
       </c>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>194</v>
+        <v>80</v>
       </c>
       <c r="B83" t="s">
+        <v>103</v>
+      </c>
+      <c r="C83" t="s">
+        <v>37</v>
+      </c>
+      <c r="D83" t="s">
+        <v>22</v>
+      </c>
+      <c r="E83" t="s">
+        <v>23</v>
+      </c>
+      <c r="F83" s="1">
+        <v>0</v>
+      </c>
+      <c r="G83" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="C83" t="s">
-        <v>21</v>
-      </c>
-      <c r="D83" t="s">
-        <v>65</v>
-      </c>
-      <c r="E83" t="s">
-        <v>23</v>
-      </c>
-      <c r="F83" s="1">
+      <c r="H83" s="1" t="str">
+        <f>IF(F83=0,G83,F83*12)</f>
+        <v xml:space="preserve"> $500-1000 </v>
+      </c>
+      <c r="I83" t="s">
         <v>5</v>
       </c>
-      <c r="G83" s="1">
-        <v>0</v>
-      </c>
-      <c r="H83" s="1">
-        <f t="shared" si="1"/>
-        <v>60</v>
-      </c>
-      <c r="I83" t="s">
-        <v>3</v>
-      </c>
       <c r="J83" t="s">
-        <v>203</v>
-      </c>
-      <c r="K83" s="1" t="s">
-        <v>261</v>
+        <v>105</v>
       </c>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>194</v>
+        <v>80</v>
       </c>
       <c r="B84" t="s">
-        <v>204</v>
+        <v>109</v>
       </c>
       <c r="C84" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="D84" t="s">
-        <v>65</v>
+        <v>22</v>
       </c>
       <c r="E84" t="s">
         <v>23</v>
@@ -4346,68 +4315,68 @@
       <c r="F84" s="1">
         <v>0</v>
       </c>
-      <c r="G84" s="1">
-        <v>1000</v>
-      </c>
-      <c r="H84" s="1">
-        <f t="shared" si="1"/>
-        <v>1000</v>
+      <c r="G84" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="H84" s="1" t="str">
+        <f>IF(F84=0,G84,F84*12)</f>
+        <v xml:space="preserve"> $500-1500 </v>
       </c>
       <c r="I84" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="J84" t="s">
-        <v>205</v>
+        <v>110</v>
       </c>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>194</v>
+        <v>111</v>
       </c>
       <c r="B85" t="s">
-        <v>206</v>
+        <v>112</v>
       </c>
       <c r="C85" t="s">
         <v>21</v>
       </c>
       <c r="D85" t="s">
-        <v>65</v>
+        <v>22</v>
       </c>
       <c r="E85" t="s">
-        <v>23</v>
+        <v>113</v>
       </c>
       <c r="F85" s="1">
-        <v>0</v>
+        <v>49</v>
       </c>
       <c r="G85" s="1">
         <v>0</v>
       </c>
       <c r="H85" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>IF(F85=0,G85,F85*12)</f>
+        <v>588</v>
       </c>
       <c r="I85" t="s">
         <v>5</v>
       </c>
       <c r="J85" t="s">
-        <v>256</v>
+        <v>114</v>
       </c>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>194</v>
+        <v>111</v>
       </c>
       <c r="B86" t="s">
-        <v>207</v>
+        <v>115</v>
       </c>
       <c r="C86" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="D86" t="s">
-        <v>65</v>
+        <v>22</v>
       </c>
       <c r="E86" t="s">
-        <v>23</v>
+        <v>113</v>
       </c>
       <c r="F86" s="1">
         <v>0</v>
@@ -4416,22 +4385,22 @@
         <v>0</v>
       </c>
       <c r="H86" s="1">
-        <f t="shared" si="1"/>
+        <f>IF(F86=0,G86,F86*12)</f>
         <v>0</v>
       </c>
       <c r="I86" t="s">
         <v>5</v>
       </c>
       <c r="J86" t="s">
-        <v>208</v>
+        <v>116</v>
       </c>
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>209</v>
+        <v>111</v>
       </c>
       <c r="B87" t="s">
-        <v>210</v>
+        <v>119</v>
       </c>
       <c r="C87" t="s">
         <v>21</v>
@@ -4440,37 +4409,37 @@
         <v>22</v>
       </c>
       <c r="E87" t="s">
-        <v>23</v>
+        <v>120</v>
       </c>
       <c r="F87" s="1">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="G87" s="1">
         <v>0</v>
       </c>
       <c r="H87" s="1">
-        <f t="shared" si="1"/>
-        <v>120</v>
+        <f>IF(F87=0,G87,F87*12)</f>
+        <v>180</v>
       </c>
       <c r="I87" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="J87" t="s">
-        <v>211</v>
+        <v>121</v>
       </c>
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>209</v>
+        <v>124</v>
       </c>
       <c r="B88" t="s">
-        <v>212</v>
+        <v>125</v>
       </c>
       <c r="C88" t="s">
         <v>21</v>
       </c>
       <c r="D88" t="s">
-        <v>65</v>
+        <v>22</v>
       </c>
       <c r="E88" t="s">
         <v>23</v>
@@ -4482,22 +4451,22 @@
         <v>0</v>
       </c>
       <c r="H88" s="1">
-        <f t="shared" si="1"/>
+        <f>IF(F88=0,G88,F88*12)</f>
         <v>0</v>
       </c>
       <c r="I88" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="J88" t="s">
-        <v>213</v>
+        <v>126</v>
       </c>
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>209</v>
+        <v>137</v>
       </c>
       <c r="B89" t="s">
-        <v>214</v>
+        <v>148</v>
       </c>
       <c r="C89" t="s">
         <v>37</v>
@@ -4508,35 +4477,35 @@
       <c r="E89" t="s">
         <v>23</v>
       </c>
-      <c r="F89" s="1">
-        <v>0</v>
+      <c r="F89" s="1" t="s">
+        <v>149</v>
       </c>
       <c r="G89" s="1">
         <v>0</v>
       </c>
-      <c r="H89" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="H89" s="1" t="e">
+        <f>IF(F89=0,G89,F89*12)</f>
+        <v>#VALUE!</v>
       </c>
       <c r="I89" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="J89" t="s">
-        <v>215</v>
+        <v>150</v>
       </c>
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>209</v>
+        <v>137</v>
       </c>
       <c r="B90" t="s">
-        <v>216</v>
+        <v>157</v>
       </c>
       <c r="C90" t="s">
         <v>21</v>
       </c>
       <c r="D90" t="s">
-        <v>65</v>
+        <v>22</v>
       </c>
       <c r="E90" t="s">
         <v>23</v>
@@ -4544,95 +4513,93 @@
       <c r="F90" s="1">
         <v>0</v>
       </c>
-      <c r="G90" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="H90" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve"> $500-1000 </v>
+      <c r="G90" s="1">
+        <v>1500</v>
+      </c>
+      <c r="H90" s="1">
+        <f>IF(F90=0,G90,F90*12)</f>
+        <v>1500</v>
       </c>
       <c r="I90" t="s">
         <v>5</v>
       </c>
       <c r="J90" t="s">
-        <v>218</v>
+        <v>158</v>
       </c>
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>209</v>
+        <v>137</v>
       </c>
       <c r="B91" t="s">
-        <v>219</v>
+        <v>162</v>
       </c>
       <c r="C91" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="D91" t="s">
-        <v>65</v>
+        <v>22</v>
       </c>
       <c r="E91" t="s">
         <v>23</v>
       </c>
-      <c r="F91" s="1">
-        <v>0</v>
-      </c>
-      <c r="G91" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="H91" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve"> $500-1000 </v>
+      <c r="F91" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="G91" s="1">
+        <v>0</v>
+      </c>
+      <c r="H91" s="1" t="e">
+        <f>IF(F91=0,G91,F91*12)</f>
+        <v>#VALUE!</v>
       </c>
       <c r="I91" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="J91" t="s">
-        <v>220</v>
+        <v>163</v>
       </c>
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>221</v>
+        <v>137</v>
       </c>
       <c r="B92" t="s">
-        <v>222</v>
+        <v>170</v>
       </c>
       <c r="C92" t="s">
         <v>21</v>
       </c>
       <c r="D92" t="s">
-        <v>65</v>
+        <v>22</v>
       </c>
       <c r="E92" t="s">
         <v>23</v>
       </c>
       <c r="F92" s="1">
-        <v>0</v>
-      </c>
-      <c r="G92" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="H92" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve"> $1500-2000 </v>
+        <v>50</v>
+      </c>
+      <c r="G92" s="1"/>
+      <c r="H92" s="1">
+        <f>IF(F92=0,G92,F92*12)</f>
+        <v>600</v>
       </c>
       <c r="I92" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="J92" t="s">
-        <v>224</v>
+        <v>171</v>
       </c>
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>221</v>
+        <v>137</v>
       </c>
       <c r="B93" t="s">
-        <v>225</v>
+        <v>172</v>
       </c>
       <c r="C93" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="D93" t="s">
         <v>22</v>
@@ -4640,29 +4607,29 @@
       <c r="E93" t="s">
         <v>23</v>
       </c>
-      <c r="F93" s="1">
-        <v>0</v>
+      <c r="F93" s="1" t="s">
+        <v>173</v>
       </c>
       <c r="G93" s="1">
         <v>0</v>
       </c>
-      <c r="H93" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="H93" s="1" t="e">
+        <f>IF(F93=0,G93,F93*12)</f>
+        <v>#VALUE!</v>
       </c>
       <c r="I93" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="J93" t="s">
-        <v>226</v>
+        <v>174</v>
       </c>
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>221</v>
+        <v>179</v>
       </c>
       <c r="B94" t="s">
-        <v>227</v>
+        <v>180</v>
       </c>
       <c r="C94" t="s">
         <v>21</v>
@@ -4673,35 +4640,36 @@
       <c r="E94" t="s">
         <v>23</v>
       </c>
-      <c r="F94" s="1">
-        <v>0</v>
+      <c r="F94" s="1" t="s">
+        <v>181</v>
       </c>
       <c r="G94" s="1">
         <v>0</v>
       </c>
-      <c r="H94" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="H94" s="1" t="e">
+        <f>IF(F94=0,G94,F94*12)</f>
+        <v>#VALUE!</v>
       </c>
       <c r="I94" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="J94" t="s">
-        <v>228</v>
-      </c>
+        <v>182</v>
+      </c>
+      <c r="K94" s="1"/>
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>221</v>
+        <v>179</v>
       </c>
       <c r="B95" t="s">
-        <v>229</v>
+        <v>183</v>
       </c>
       <c r="C95" t="s">
         <v>21</v>
       </c>
       <c r="D95" t="s">
-        <v>22</v>
+        <v>65</v>
       </c>
       <c r="E95" t="s">
         <v>23</v>
@@ -4713,28 +4681,28 @@
         <v>0</v>
       </c>
       <c r="H95" s="1">
-        <f t="shared" si="1"/>
+        <f>IF(F95=0,G95,F95*12)</f>
         <v>0</v>
       </c>
       <c r="I95" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="J95" t="s">
-        <v>230</v>
+        <v>184</v>
       </c>
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>221</v>
+        <v>179</v>
       </c>
       <c r="B96" t="s">
-        <v>231</v>
+        <v>191</v>
       </c>
       <c r="C96" t="s">
         <v>21</v>
       </c>
       <c r="D96" t="s">
-        <v>22</v>
+        <v>65</v>
       </c>
       <c r="E96" t="s">
         <v>23</v>
@@ -4746,61 +4714,61 @@
         <v>0</v>
       </c>
       <c r="H96" s="1">
-        <f t="shared" si="1"/>
+        <f>IF(F96=0,G96,F96*12)</f>
         <v>0</v>
       </c>
       <c r="I96" t="s">
         <v>5</v>
       </c>
       <c r="J96" t="s">
-        <v>232</v>
+        <v>241</v>
       </c>
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>221</v>
+        <v>179</v>
       </c>
       <c r="B97" t="s">
-        <v>233</v>
+        <v>192</v>
       </c>
       <c r="C97" t="s">
         <v>21</v>
       </c>
       <c r="D97" t="s">
-        <v>22</v>
+        <v>65</v>
       </c>
       <c r="E97" t="s">
-        <v>128</v>
+        <v>23</v>
       </c>
       <c r="F97" s="1">
-        <v>99</v>
+        <v>0</v>
       </c>
       <c r="G97" s="1">
-        <v>1188</v>
+        <v>0</v>
       </c>
       <c r="H97" s="1">
-        <f t="shared" si="1"/>
-        <v>1188</v>
+        <f>IF(F97=0,G97,F97*12)</f>
+        <v>0</v>
       </c>
       <c r="I97" t="s">
         <v>5</v>
       </c>
       <c r="J97" t="s">
-        <v>234</v>
+        <v>193</v>
       </c>
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>235</v>
+        <v>194</v>
       </c>
       <c r="B98" t="s">
-        <v>236</v>
+        <v>201</v>
       </c>
       <c r="C98" t="s">
         <v>21</v>
       </c>
       <c r="D98" t="s">
-        <v>22</v>
+        <v>65</v>
       </c>
       <c r="E98" t="s">
         <v>23</v>
@@ -4808,35 +4776,35 @@
       <c r="F98" s="1">
         <v>0</v>
       </c>
-      <c r="G98" s="1">
-        <v>0</v>
-      </c>
-      <c r="H98" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="G98" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="H98" s="1" t="str">
+        <f>IF(F98=0,G98,F98*12)</f>
+        <v xml:space="preserve"> $500-1000 </v>
       </c>
       <c r="I98" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="J98" t="s">
-        <v>237</v>
+        <v>203</v>
       </c>
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>235</v>
+        <v>206</v>
       </c>
       <c r="B99" t="s">
-        <v>238</v>
+        <v>216</v>
       </c>
       <c r="C99" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="D99" t="s">
         <v>22</v>
       </c>
       <c r="E99" t="s">
-        <v>239</v>
+        <v>23</v>
       </c>
       <c r="F99" s="1">
         <v>0</v>
@@ -4845,216 +4813,84 @@
         <v>0</v>
       </c>
       <c r="H99" s="1">
-        <f t="shared" si="1"/>
+        <f>IF(F99=0,G99,F99*12)</f>
         <v>0</v>
       </c>
       <c r="I99" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="J99" t="s">
-        <v>240</v>
+        <v>217</v>
       </c>
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>235</v>
+        <v>206</v>
       </c>
       <c r="B100" t="s">
-        <v>241</v>
+        <v>218</v>
       </c>
       <c r="C100" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="D100" t="s">
         <v>22</v>
       </c>
       <c r="E100" t="s">
-        <v>23</v>
+        <v>113</v>
       </c>
       <c r="F100" s="1">
-        <v>0</v>
+        <v>99</v>
       </c>
       <c r="G100" s="1">
-        <v>0</v>
+        <v>1188</v>
       </c>
       <c r="H100" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>IF(F100=0,G100,F100*12)</f>
+        <v>1188</v>
       </c>
       <c r="I100" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="J100" t="s">
-        <v>242</v>
+        <v>219</v>
       </c>
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
+        <v>231</v>
+      </c>
+      <c r="B101" t="s">
+        <v>234</v>
+      </c>
+      <c r="C101" t="s">
+        <v>21</v>
+      </c>
+      <c r="D101" t="s">
+        <v>22</v>
+      </c>
+      <c r="E101" t="s">
+        <v>23</v>
+      </c>
+      <c r="F101" s="1">
+        <v>0</v>
+      </c>
+      <c r="G101" s="1">
+        <v>100</v>
+      </c>
+      <c r="H101" s="1">
+        <f>IF(F101=0,G101,F101*12)</f>
+        <v>100</v>
+      </c>
+      <c r="I101" t="s">
+        <v>5</v>
+      </c>
+      <c r="J101" t="s">
         <v>235</v>
       </c>
-      <c r="B101" t="s">
-        <v>243</v>
-      </c>
-      <c r="C101" t="s">
-        <v>37</v>
-      </c>
-      <c r="D101" t="s">
-        <v>22</v>
-      </c>
-      <c r="E101" t="s">
-        <v>244</v>
-      </c>
-      <c r="F101" s="1">
-        <v>0</v>
-      </c>
-      <c r="G101" s="1">
-        <v>0</v>
-      </c>
-      <c r="H101" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I101" t="s">
-        <v>7</v>
-      </c>
-      <c r="J101" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A102" t="s">
-        <v>246</v>
-      </c>
-      <c r="B102" t="s">
-        <v>247</v>
-      </c>
-      <c r="C102" t="s">
-        <v>21</v>
-      </c>
-      <c r="D102" t="s">
-        <v>22</v>
-      </c>
-      <c r="E102" t="s">
-        <v>23</v>
-      </c>
-      <c r="F102" s="1">
-        <v>0</v>
-      </c>
-      <c r="G102" s="1">
-        <v>2000</v>
-      </c>
-      <c r="H102" s="1">
-        <f t="shared" si="1"/>
-        <v>2000</v>
-      </c>
-      <c r="I102" t="s">
-        <v>7</v>
-      </c>
-      <c r="J102" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A103" t="s">
-        <v>246</v>
-      </c>
-      <c r="B103" t="s">
-        <v>249</v>
-      </c>
-      <c r="C103" t="s">
-        <v>21</v>
-      </c>
-      <c r="D103" t="s">
-        <v>22</v>
-      </c>
-      <c r="E103" t="s">
-        <v>23</v>
-      </c>
-      <c r="F103" s="1">
-        <v>0</v>
-      </c>
-      <c r="G103" s="1">
-        <v>100</v>
-      </c>
-      <c r="H103" s="1">
-        <f t="shared" si="1"/>
-        <v>100</v>
-      </c>
-      <c r="I103" t="s">
-        <v>5</v>
-      </c>
-      <c r="J103" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A104" t="s">
-        <v>251</v>
-      </c>
-      <c r="B104" t="s">
-        <v>252</v>
-      </c>
-      <c r="C104" t="s">
-        <v>37</v>
-      </c>
-      <c r="D104" t="s">
-        <v>22</v>
-      </c>
-      <c r="E104" t="s">
-        <v>23</v>
-      </c>
-      <c r="F104" s="1">
-        <v>0</v>
-      </c>
-      <c r="G104" s="1">
-        <v>0</v>
-      </c>
-      <c r="H104" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I104" t="s">
-        <v>7</v>
-      </c>
-      <c r="J104" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A105" t="s">
-        <v>251</v>
-      </c>
-      <c r="B105" t="s">
-        <v>254</v>
-      </c>
-      <c r="C105" t="s">
-        <v>21</v>
-      </c>
-      <c r="D105" t="s">
-        <v>22</v>
-      </c>
-      <c r="E105" t="s">
-        <v>23</v>
-      </c>
-      <c r="F105" s="1">
-        <v>0</v>
-      </c>
-      <c r="G105" s="1">
-        <v>200</v>
-      </c>
-      <c r="H105" s="1">
-        <f t="shared" si="1"/>
-        <v>200</v>
-      </c>
-      <c r="I105" t="s">
-        <v>7</v>
-      </c>
-      <c r="J105" t="s">
-        <v>255</v>
-      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A7:K105" xr:uid="{C78ECC95-93BA-E742-8CDF-F456D018CBC0}"/>
+  <autoFilter ref="A7:K101" xr:uid="{C78ECC95-93BA-E742-8CDF-F456D018CBC0}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>